<commit_message>
error in SNOW_crocus corrected
</commit_message>
<xml_diff>
--- a/param_file_templates/Excel/GROUND_freeW_bucketW_seb_snow.xlsx
+++ b/param_file_templates/Excel/GROUND_freeW_bucketW_seb_snow.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD44"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>